<commit_message>
Sorted activities on wbs_id
Activities are now shown in right order in xls
Project activity added
</commit_message>
<xml_diff>
--- a/PMConverter/src/test_alexander.xlsx
+++ b/PMConverter/src/test_alexander.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="206">
   <si>
     <t>General</t>
   </si>
@@ -72,6 +72,21 @@
     <t>Total Cost</t>
   </si>
   <si>
+    <t>Claeys-Verhelst Premises</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10d </t>
+  </si>
+  <si>
+    <t>preparation</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
     <t>building permit</t>
   </si>
   <si>
@@ -111,6 +126,15 @@
     <t>1.1.4</t>
   </si>
   <si>
+    <t>preparation contractor</t>
+  </si>
+  <si>
+    <t>1.1.5</t>
+  </si>
+  <si>
+    <t>FS6+0</t>
+  </si>
+  <si>
     <t>demolition</t>
   </si>
   <si>
@@ -120,19 +144,13 @@
     <t>FS17+0;FS69+0</t>
   </si>
   <si>
-    <t xml:space="preserve">10d </t>
-  </si>
-  <si>
     <t>team VDW [4.0 #8]</t>
   </si>
   <si>
-    <t>preparation contractor</t>
-  </si>
-  <si>
-    <t>1.1.5</t>
-  </si>
-  <si>
-    <t>FS6+0</t>
+    <t>foundation</t>
+  </si>
+  <si>
+    <t>1.2</t>
   </si>
   <si>
     <t>excavation</t>
@@ -150,6 +168,18 @@
     <t>team VDW</t>
   </si>
   <si>
+    <t>soil analyses</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>FS18+0</t>
+  </si>
+  <si>
+    <t>0d 16h</t>
+  </si>
+  <si>
     <t>foundation beam</t>
   </si>
   <si>
@@ -168,6 +198,42 @@
     <t>team VDW [3.0 #8]</t>
   </si>
   <si>
+    <t>placing sewerage</t>
+  </si>
+  <si>
+    <t>1.2.4</t>
+  </si>
+  <si>
+    <t>FS17+0</t>
+  </si>
+  <si>
+    <t>FS23+0</t>
+  </si>
+  <si>
+    <t>3d 8h</t>
+  </si>
+  <si>
+    <t>foundation plate</t>
+  </si>
+  <si>
+    <t>1.2.5</t>
+  </si>
+  <si>
+    <t>FS21+0</t>
+  </si>
+  <si>
+    <t>0d 8h</t>
+  </si>
+  <si>
+    <t>team VDW [5.0 #8]</t>
+  </si>
+  <si>
+    <t>shell</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
     <t>steelframe I</t>
   </si>
   <si>
@@ -189,21 +255,6 @@
     <t>FS22+0</t>
   </si>
   <si>
-    <t>3d 8h</t>
-  </si>
-  <si>
-    <t>placing sewerage</t>
-  </si>
-  <si>
-    <t>1.2.4</t>
-  </si>
-  <si>
-    <t>FS17+0</t>
-  </si>
-  <si>
-    <t>FS23+0</t>
-  </si>
-  <si>
     <t>steelframe II</t>
   </si>
   <si>
@@ -216,21 +267,6 @@
     <t xml:space="preserve">5d </t>
   </si>
   <si>
-    <t>foundation plate</t>
-  </si>
-  <si>
-    <t>1.2.5</t>
-  </si>
-  <si>
-    <t>FS21+0</t>
-  </si>
-  <si>
-    <t>0d 8h</t>
-  </si>
-  <si>
-    <t>team VDW [5.0 #8]</t>
-  </si>
-  <si>
     <t>concrete volt II</t>
   </si>
   <si>
@@ -240,6 +276,12 @@
     <t>FS25+0;FS49+0</t>
   </si>
   <si>
+    <t>wind and water proof</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
     <t>facades</t>
   </si>
   <si>
@@ -267,25 +309,61 @@
     <t>windows [3.0 #3]</t>
   </si>
   <si>
+    <t>roof</t>
+  </si>
+  <si>
+    <t>1.4.3</t>
+  </si>
+  <si>
+    <t>roofing [4.0 #4]</t>
+  </si>
+  <si>
+    <t>warehouse</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>v0 polierbeton</t>
+  </si>
+  <si>
+    <t>1.5.1</t>
+  </si>
+  <si>
+    <t>FS30+0;FS27+0;FS59+0;FS52+0;FS45+0;FS34+0;FS60+0;FS51+0</t>
+  </si>
+  <si>
+    <t>v0 sanitary</t>
+  </si>
+  <si>
+    <t>1.5.2</t>
+  </si>
+  <si>
+    <t>31FS+0;FS28+0</t>
+  </si>
+  <si>
+    <t>FS35+0</t>
+  </si>
+  <si>
+    <t>plumber</t>
+  </si>
+  <si>
     <t>v0 -masonry</t>
   </si>
   <si>
     <t>1.5.3</t>
   </si>
   <si>
-    <t>31FS+0;FS28+0</t>
-  </si>
-  <si>
     <t>mason</t>
   </si>
   <si>
-    <t>v0 polierbeton</t>
-  </si>
-  <si>
-    <t>1.5.1</t>
-  </si>
-  <si>
-    <t>FS30+0;FS27+0;FS59+0;FS52+0;FS45+0;FS34+0;FS60+0;FS51+0</t>
+    <t>v0 heating</t>
+  </si>
+  <si>
+    <t>1.5.4</t>
+  </si>
+  <si>
+    <t>heating</t>
   </si>
   <si>
     <t>v0 electricity</t>
@@ -297,30 +375,174 @@
     <t>26FS+0;FS31+0</t>
   </si>
   <si>
-    <t>FS35+0</t>
-  </si>
-  <si>
     <t>electrician</t>
   </si>
   <si>
-    <t>v0 sanitary</t>
-  </si>
-  <si>
-    <t>1.5.2</t>
-  </si>
-  <si>
-    <t>plumber</t>
+    <t>v0 floors</t>
+  </si>
+  <si>
+    <t>1.5.6</t>
+  </si>
+  <si>
+    <t>59FS+0;29FS+0;FS30+0</t>
+  </si>
+  <si>
+    <t>FS41+0;FS37+0</t>
+  </si>
+  <si>
+    <t>flooring</t>
   </si>
   <si>
     <t>construction leave</t>
   </si>
   <si>
+    <t>1.6</t>
+  </si>
+  <si>
     <t>1.6.1</t>
   </si>
   <si>
     <t>FS53+0;FS55+0;FS56+0;FS61+0;FS54+0;FS30+0;FS27+0;FS59+0;FS52+0;FS45+0;FS34+0;FS60+0;FS51+0;FS29+0</t>
   </si>
   <si>
+    <t>level 1</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>vI sanitary</t>
+  </si>
+  <si>
+    <t>1.7.1</t>
+  </si>
+  <si>
+    <t>vI masonry</t>
+  </si>
+  <si>
+    <t>1.7.2</t>
+  </si>
+  <si>
+    <t>v1screed</t>
+  </si>
+  <si>
+    <t>1.7.3</t>
+  </si>
+  <si>
+    <t>FS67+0</t>
+  </si>
+  <si>
+    <t>chapen [2.0 #3]</t>
+  </si>
+  <si>
+    <t>v1 heating</t>
+  </si>
+  <si>
+    <t>1.7.4</t>
+  </si>
+  <si>
+    <t>vI electricity</t>
+  </si>
+  <si>
+    <t>1.7.5</t>
+  </si>
+  <si>
+    <t>v1 drying screed</t>
+  </si>
+  <si>
+    <t>1.7.6</t>
+  </si>
+  <si>
+    <t>FS34+0</t>
+  </si>
+  <si>
+    <t>FS57+0;FS32+0</t>
+  </si>
+  <si>
+    <t>1d 16h</t>
+  </si>
+  <si>
+    <t>v1flooring</t>
+  </si>
+  <si>
+    <t>1.7.7</t>
+  </si>
+  <si>
+    <t>FS41+0;FS37+0;FS36+0</t>
+  </si>
+  <si>
+    <t>level 2</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>v2 sanitary</t>
+  </si>
+  <si>
+    <t>1.8.1</t>
+  </si>
+  <si>
+    <t>FS31+0</t>
+  </si>
+  <si>
+    <t>v2 masonry</t>
+  </si>
+  <si>
+    <t>1.8.2</t>
+  </si>
+  <si>
+    <t>v2 screed</t>
+  </si>
+  <si>
+    <t>1.8.3</t>
+  </si>
+  <si>
+    <t>FS68+0;FS36+0</t>
+  </si>
+  <si>
+    <t>chapen</t>
+  </si>
+  <si>
+    <t>v2 heating</t>
+  </si>
+  <si>
+    <t>1.8.4</t>
+  </si>
+  <si>
+    <t>v2 electricity</t>
+  </si>
+  <si>
+    <t>1.8.5</t>
+  </si>
+  <si>
+    <t>v2 drying screed</t>
+  </si>
+  <si>
+    <t>1.8.6</t>
+  </si>
+  <si>
+    <t>FS56+0</t>
+  </si>
+  <si>
+    <t>FS58+0;FS32+0</t>
+  </si>
+  <si>
+    <t>v2 flooring</t>
+  </si>
+  <si>
+    <t>1.8.7</t>
+  </si>
+  <si>
+    <t>FS68+0</t>
+  </si>
+  <si>
+    <t>completion</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
     <t>stucco</t>
   </si>
   <si>
@@ -330,36 +552,9 @@
     <t>68FS+0;FS67+0</t>
   </si>
   <si>
-    <t>FS41+0;FS37+0</t>
-  </si>
-  <si>
     <t>stucco [3.0 #4]</t>
   </si>
   <si>
-    <t>v1screed</t>
-  </si>
-  <si>
-    <t>1.7.3</t>
-  </si>
-  <si>
-    <t>FS67+0</t>
-  </si>
-  <si>
-    <t>chapen [2.0 #3]</t>
-  </si>
-  <si>
-    <t>v0 floors</t>
-  </si>
-  <si>
-    <t>1.5.6</t>
-  </si>
-  <si>
-    <t>59FS+0;29FS+0;FS30+0</t>
-  </si>
-  <si>
-    <t>flooring</t>
-  </si>
-  <si>
     <t>drywall</t>
   </si>
   <si>
@@ -369,33 +564,54 @@
     <t>58FS+0;57FS+0;FS56+0</t>
   </si>
   <si>
+    <t>kitchen and bar</t>
+  </si>
+  <si>
+    <t>1.9.3</t>
+  </si>
+  <si>
+    <t>32FS+0;58FS+0;57FS+0;FS35+0</t>
+  </si>
+  <si>
     <t>techniques</t>
   </si>
   <si>
     <t>1.9.4</t>
   </si>
   <si>
-    <t>32FS+0;58FS+0;57FS+0;FS35+0</t>
-  </si>
-  <si>
     <t>FS38+0;FS42+0;FS43+0;FS44+0</t>
   </si>
   <si>
+    <t>stairs</t>
+  </si>
+  <si>
+    <t>1.9.5</t>
+  </si>
+  <si>
+    <t>FS37+0</t>
+  </si>
+  <si>
+    <t>entrance doors</t>
+  </si>
+  <si>
+    <t>1.9.6</t>
+  </si>
+  <si>
+    <t>elevator</t>
+  </si>
+  <si>
+    <t>1.9.7</t>
+  </si>
+  <si>
     <t>suspended ceiling</t>
   </si>
   <si>
     <t>1.9.8</t>
   </si>
   <si>
-    <t>FS37+0</t>
-  </si>
-  <si>
     <t>FS39+0</t>
   </si>
   <si>
-    <t>1d 16h</t>
-  </si>
-  <si>
     <t>painting</t>
   </si>
   <si>
@@ -418,216 +634,6 @@
   </si>
   <si>
     <t>furniture [5.0 #5]</t>
-  </si>
-  <si>
-    <t>kitchen and bar</t>
-  </si>
-  <si>
-    <t>1.9.3</t>
-  </si>
-  <si>
-    <t>entrance doors</t>
-  </si>
-  <si>
-    <t>1.9.6</t>
-  </si>
-  <si>
-    <t>elevator</t>
-  </si>
-  <si>
-    <t>1.9.7</t>
-  </si>
-  <si>
-    <t>stairs</t>
-  </si>
-  <si>
-    <t>1.9.5</t>
-  </si>
-  <si>
-    <t>vI masonry</t>
-  </si>
-  <si>
-    <t>1.7.2</t>
-  </si>
-  <si>
-    <t>preparation</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>foundation</t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>shell</t>
-  </si>
-  <si>
-    <t>1.3</t>
-  </si>
-  <si>
-    <t>roof</t>
-  </si>
-  <si>
-    <t>1.4.3</t>
-  </si>
-  <si>
-    <t>roofing [4.0 #4]</t>
-  </si>
-  <si>
-    <t>wind and water proof</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>vI electricity</t>
-  </si>
-  <si>
-    <t>1.7.5</t>
-  </si>
-  <si>
-    <t>vI sanitary</t>
-  </si>
-  <si>
-    <t>1.7.1</t>
-  </si>
-  <si>
-    <t>v2 sanitary</t>
-  </si>
-  <si>
-    <t>1.8.1</t>
-  </si>
-  <si>
-    <t>FS31+0</t>
-  </si>
-  <si>
-    <t>v2 electricity</t>
-  </si>
-  <si>
-    <t>1.8.5</t>
-  </si>
-  <si>
-    <t>v2 masonry</t>
-  </si>
-  <si>
-    <t>1.8.2</t>
-  </si>
-  <si>
-    <t>v2 screed</t>
-  </si>
-  <si>
-    <t>1.8.3</t>
-  </si>
-  <si>
-    <t>FS68+0;FS36+0</t>
-  </si>
-  <si>
-    <t>chapen</t>
-  </si>
-  <si>
-    <t>v1flooring</t>
-  </si>
-  <si>
-    <t>1.7.7</t>
-  </si>
-  <si>
-    <t>FS41+0;FS37+0;FS36+0</t>
-  </si>
-  <si>
-    <t>v2 flooring</t>
-  </si>
-  <si>
-    <t>1.8.7</t>
-  </si>
-  <si>
-    <t>FS68+0</t>
-  </si>
-  <si>
-    <t>v0 heating</t>
-  </si>
-  <si>
-    <t>1.5.4</t>
-  </si>
-  <si>
-    <t>heating</t>
-  </si>
-  <si>
-    <t>v1 heating</t>
-  </si>
-  <si>
-    <t>1.7.4</t>
-  </si>
-  <si>
-    <t>v2 heating</t>
-  </si>
-  <si>
-    <t>1.8.4</t>
-  </si>
-  <si>
-    <t>warehouse</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>level 1</t>
-  </si>
-  <si>
-    <t>1.7</t>
-  </si>
-  <si>
-    <t>level 2</t>
-  </si>
-  <si>
-    <t>1.8</t>
-  </si>
-  <si>
-    <t>completion</t>
-  </si>
-  <si>
-    <t>1.9</t>
-  </si>
-  <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t>v1 drying screed</t>
-  </si>
-  <si>
-    <t>1.7.6</t>
-  </si>
-  <si>
-    <t>FS34+0</t>
-  </si>
-  <si>
-    <t>FS57+0;FS32+0</t>
-  </si>
-  <si>
-    <t>v2 drying screed</t>
-  </si>
-  <si>
-    <t>1.8.6</t>
-  </si>
-  <si>
-    <t>FS56+0</t>
-  </si>
-  <si>
-    <t>FS58+0;FS32+0</t>
-  </si>
-  <si>
-    <t>soil analyses</t>
-  </si>
-  <si>
-    <t>1.2.2</t>
-  </si>
-  <si>
-    <t>FS18+0</t>
-  </si>
-  <si>
-    <t>0d 16h</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1032,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N60"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1116,7 +1122,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>18</v>
@@ -1125,24 +1131,22 @@
         <v>19</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="4">
+        <v>42116.4652200366</v>
+      </c>
+      <c r="G3" s="4">
+        <v>42126.4652200368</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="F3" s="4">
-        <v>38824.3333333333</v>
-      </c>
-      <c r="G3" s="4">
-        <v>42125.9500275435</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="5">
         <v>0</v>
       </c>
       <c r="K3" s="5">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="L3" s="5">
         <v>0</v>
@@ -1151,40 +1155,36 @@
         <v>0</v>
       </c>
       <c r="N3" s="5">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="4">
-        <v>38908.3333333333</v>
+        <v>42116.4652200366</v>
       </c>
       <c r="G4" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="5">
         <v>0</v>
       </c>
       <c r="K4" s="5">
-        <v>210000</v>
+        <v>0</v>
       </c>
       <c r="L4" s="5">
         <v>0</v>
@@ -1193,26 +1193,28 @@
         <v>0</v>
       </c>
       <c r="N4" s="5">
-        <v>210000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F5" s="4">
         <v>38824.3333333333</v>
       </c>
       <c r="G5" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>26</v>
@@ -1222,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="5">
-        <v>3765.31005859375</v>
+        <v>75</v>
       </c>
       <c r="L5" s="5">
         <v>0</v>
@@ -1231,36 +1233,40 @@
         <v>0</v>
       </c>
       <c r="N5" s="5">
-        <v>3765.31005859375</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
       <c r="F6" s="4">
-        <v>38824.3333333333</v>
+        <v>38908.3333333333</v>
       </c>
       <c r="G6" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="5">
         <v>0</v>
       </c>
       <c r="K6" s="5">
-        <v>1876.5400390625</v>
+        <v>210000</v>
       </c>
       <c r="L6" s="5">
         <v>0</v>
@@ -1269,42 +1275,36 @@
         <v>0</v>
       </c>
       <c r="N6" s="5">
-        <v>1876.5400390625</v>
+        <v>210000</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4">
+        <v>38824.3333333333</v>
+      </c>
+      <c r="G7" s="4">
+        <v>42126.4652200368</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="4">
-        <v>39020.3333333333</v>
-      </c>
-      <c r="G7" s="4">
-        <v>42125.9500275435</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="I7" s="3"/>
       <c r="J7" s="5">
-        <v>12339.2</v>
+        <v>0</v>
       </c>
       <c r="K7" s="5">
-        <v>1070.10998535156</v>
+        <v>3765.31005859375</v>
       </c>
       <c r="L7" s="5">
         <v>0</v>
@@ -1313,40 +1313,36 @@
         <v>0</v>
       </c>
       <c r="N7" s="5">
-        <v>13409.3099853516</v>
+        <v>3765.31005859375</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>38</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="4">
-        <v>38936.3333333333</v>
+        <v>38824.3333333333</v>
       </c>
       <c r="G8" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="5">
         <v>0</v>
       </c>
       <c r="K8" s="5">
-        <v>0.00999999977648258</v>
+        <v>1876.5400390625</v>
       </c>
       <c r="L8" s="5">
         <v>0</v>
@@ -1355,42 +1351,40 @@
         <v>0</v>
       </c>
       <c r="N8" s="5">
-        <v>0.00999999977648258</v>
+        <v>1876.5400390625</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="F9" s="4">
-        <v>39062.3333333333</v>
+        <v>38936.3333333333</v>
       </c>
       <c r="G9" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>43</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="I9" s="3"/>
       <c r="J9" s="5">
-        <v>1850.88</v>
+        <v>0</v>
       </c>
       <c r="K9" s="5">
-        <v>26000</v>
+        <v>0.00999999977648258</v>
       </c>
       <c r="L9" s="5">
         <v>0</v>
@@ -1399,42 +1393,42 @@
         <v>0</v>
       </c>
       <c r="N9" s="5">
-        <v>27850.88</v>
+        <v>0.00999999977648258</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F10" s="4">
-        <v>39080.3333333333</v>
+        <v>39020.3333333333</v>
       </c>
       <c r="G10" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="J10" s="5">
-        <v>8328.96</v>
+        <v>12339.2</v>
       </c>
       <c r="K10" s="5">
-        <v>98523.7265625</v>
+        <v>1070.10998535156</v>
       </c>
       <c r="L10" s="5">
         <v>0</v>
@@ -1443,42 +1437,36 @@
         <v>0</v>
       </c>
       <c r="N10" s="5">
-        <v>106852.6865625</v>
+        <v>13409.3099853516</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>53</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="4">
-        <v>39115.3333333333</v>
+        <v>42116.4652200366</v>
       </c>
       <c r="G11" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I11" s="3"/>
       <c r="J11" s="5">
-        <v>9871.36</v>
+        <v>0</v>
       </c>
       <c r="K11" s="5">
-        <v>118992.5078125</v>
+        <v>0</v>
       </c>
       <c r="L11" s="5">
         <v>0</v>
@@ -1487,42 +1475,42 @@
         <v>0</v>
       </c>
       <c r="N11" s="5">
-        <v>128863.8678125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="2">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="F12" s="4">
-        <v>39143.3333333333</v>
+        <v>39062.3333333333</v>
       </c>
       <c r="G12" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="J12" s="5">
-        <v>4935.68</v>
+        <v>1850.88</v>
       </c>
       <c r="K12" s="5">
-        <v>117409.71875</v>
+        <v>26000</v>
       </c>
       <c r="L12" s="5">
         <v>0</v>
@@ -1531,42 +1519,42 @@
         <v>0</v>
       </c>
       <c r="N12" s="5">
-        <v>122345.39875</v>
+        <v>27850.88</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F13" s="4">
-        <v>39080.3333333333</v>
+        <v>39062.3333333333</v>
       </c>
       <c r="G13" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>49</v>
       </c>
       <c r="J13" s="5">
-        <v>3701.76</v>
+        <v>616.96</v>
       </c>
       <c r="K13" s="5">
-        <v>1224.72998046875</v>
+        <v>2000</v>
       </c>
       <c r="L13" s="5">
         <v>0</v>
@@ -1575,42 +1563,42 @@
         <v>0</v>
       </c>
       <c r="N13" s="5">
-        <v>4926.48998046875</v>
+        <v>2616.96</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F14" s="4">
-        <v>39157.3333333333</v>
+        <v>39080.3333333333</v>
       </c>
       <c r="G14" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="J14" s="5">
-        <v>4627.2</v>
+        <v>8328.96</v>
       </c>
       <c r="K14" s="5">
-        <v>118992.5078125</v>
+        <v>98523.7265625</v>
       </c>
       <c r="L14" s="5">
         <v>0</v>
@@ -1619,42 +1607,42 @@
         <v>0</v>
       </c>
       <c r="N14" s="5">
-        <v>123619.7078125</v>
+        <v>106852.6865625</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="F15" s="4">
-        <v>39094.3333333333</v>
+        <v>39080.3333333333</v>
       </c>
       <c r="G15" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="J15" s="5">
-        <v>1542.4</v>
+        <v>3701.76</v>
       </c>
       <c r="K15" s="5">
-        <v>234819.4375</v>
+        <v>1224.72998046875</v>
       </c>
       <c r="L15" s="5">
         <v>0</v>
@@ -1663,42 +1651,42 @@
         <v>0</v>
       </c>
       <c r="N15" s="5">
-        <v>236361.8375</v>
+        <v>4926.48998046875</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F16" s="4">
-        <v>39178.3333333333</v>
+        <v>39094.3333333333</v>
       </c>
       <c r="G16" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="J16" s="5">
-        <v>6169.6</v>
+        <v>1542.4</v>
       </c>
       <c r="K16" s="5">
-        <v>117409.71875</v>
+        <v>234819.4375</v>
       </c>
       <c r="L16" s="5">
         <v>0</v>
@@ -1707,42 +1695,36 @@
         <v>0</v>
       </c>
       <c r="N16" s="5">
-        <v>123579.31875</v>
+        <v>236361.8375</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="2">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>76</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="4">
-        <v>39199.3333333333</v>
+        <v>42116.4652200366</v>
       </c>
       <c r="G17" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>77</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I17" s="3"/>
       <c r="J17" s="5">
-        <v>4935.68</v>
+        <v>0</v>
       </c>
       <c r="K17" s="5">
-        <v>339314</v>
+        <v>0</v>
       </c>
       <c r="L17" s="5">
         <v>0</v>
@@ -1751,42 +1733,42 @@
         <v>0</v>
       </c>
       <c r="N17" s="5">
-        <v>344249.68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F18" s="4">
-        <v>39227.3333333333</v>
+        <v>39115.3333333333</v>
       </c>
       <c r="G18" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="J18" s="5">
-        <v>3648</v>
+        <v>9871.36</v>
       </c>
       <c r="K18" s="5">
-        <v>150750.59375</v>
+        <v>118992.5078125</v>
       </c>
       <c r="L18" s="5">
         <v>0</v>
@@ -1795,84 +1777,86 @@
         <v>0</v>
       </c>
       <c r="N18" s="5">
-        <v>154398.59375</v>
+        <v>128863.8678125</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="F19" s="4">
-        <v>39323.4166666667</v>
+        <v>39143.3333333333</v>
       </c>
       <c r="G19" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="J19" s="5">
-        <v>1300.8</v>
+        <v>4935.68</v>
       </c>
       <c r="K19" s="5">
-        <v>31200.9609375</v>
+        <v>117409.71875</v>
       </c>
       <c r="L19" s="5">
-        <v>40.6500015258789</v>
+        <v>0</v>
       </c>
       <c r="M19" s="5">
-        <v>26016.0009765625</v>
+        <v>0</v>
       </c>
       <c r="N19" s="5">
-        <v>58517.7619140625</v>
+        <v>122345.39875</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F20" s="4">
-        <v>39241.3333333333</v>
+        <v>39157.3333333333</v>
       </c>
       <c r="G20" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="J20" s="5">
-        <v>6169.6</v>
+        <v>4627.2</v>
       </c>
       <c r="K20" s="5">
-        <v>134400</v>
+        <v>118992.5078125</v>
       </c>
       <c r="L20" s="5">
         <v>0</v>
@@ -1881,42 +1865,42 @@
         <v>0</v>
       </c>
       <c r="N20" s="5">
-        <v>140569.6</v>
+        <v>123619.7078125</v>
       </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="2">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="F21" s="4">
-        <v>39323.4166666667</v>
+        <v>39178.3333333333</v>
       </c>
       <c r="G21" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="J21" s="5">
-        <v>2304</v>
+        <v>6169.6</v>
       </c>
       <c r="K21" s="5">
-        <v>0</v>
+        <v>117409.71875</v>
       </c>
       <c r="L21" s="5">
         <v>0</v>
@@ -1925,42 +1909,36 @@
         <v>0</v>
       </c>
       <c r="N21" s="5">
-        <v>2304</v>
+        <v>123579.31875</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>93</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
       <c r="F22" s="4">
-        <v>39323.4166666667</v>
+        <v>42116.4652200366</v>
       </c>
       <c r="G22" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>97</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I22" s="3"/>
       <c r="J22" s="5">
-        <v>1152</v>
+        <v>0</v>
       </c>
       <c r="K22" s="5">
-        <v>4793</v>
+        <v>0</v>
       </c>
       <c r="L22" s="5">
         <v>0</v>
@@ -1969,38 +1947,42 @@
         <v>0</v>
       </c>
       <c r="N22" s="5">
-        <v>5945</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="2">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="4">
+        <v>39199.3333333333</v>
+      </c>
+      <c r="G23" s="4">
+        <v>42126.4652200368</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="4">
-        <v>39309.4166666667</v>
-      </c>
-      <c r="G23" s="4">
-        <v>42125.9500275435</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="J23" s="5">
-        <v>0</v>
+        <v>4935.68</v>
       </c>
       <c r="K23" s="5">
-        <v>0.00999999977648258</v>
+        <v>339314</v>
       </c>
       <c r="L23" s="5">
         <v>0</v>
@@ -2009,42 +1991,42 @@
         <v>0</v>
       </c>
       <c r="N23" s="5">
-        <v>0.00999999977648258</v>
+        <v>344249.68</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="2">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F24" s="4">
-        <v>39351.4166666667</v>
+        <v>39227.3333333333</v>
       </c>
       <c r="G24" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J24" s="5">
-        <v>4965.6</v>
+        <v>3648</v>
       </c>
       <c r="K24" s="5">
-        <v>8642</v>
+        <v>150750.59375</v>
       </c>
       <c r="L24" s="5">
         <v>0</v>
@@ -2053,86 +2035,78 @@
         <v>0</v>
       </c>
       <c r="N24" s="5">
-        <v>13607.6</v>
+        <v>154398.59375</v>
       </c>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="2">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>108</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="E25" s="3"/>
       <c r="F25" s="4">
-        <v>39323.4166666667</v>
+        <v>39199.3333333333</v>
       </c>
       <c r="G25" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="J25" s="5">
-        <v>0</v>
+        <v>4608</v>
       </c>
       <c r="K25" s="5">
-        <v>106140</v>
+        <v>70779.5703125</v>
       </c>
       <c r="L25" s="5">
-        <v>0</v>
+        <v>40.2999992370605</v>
       </c>
       <c r="M25" s="5">
-        <v>0</v>
+        <v>25791.9995117187</v>
       </c>
       <c r="N25" s="5">
-        <v>106140</v>
+        <v>101179.569824219</v>
       </c>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="2">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>104</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
       <c r="F26" s="4">
-        <v>39358.4166666667</v>
+        <v>42116.4652200366</v>
       </c>
       <c r="G26" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>113</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I26" s="3"/>
       <c r="J26" s="5">
-        <v>2659.84</v>
+        <v>0</v>
       </c>
       <c r="K26" s="5">
-        <v>75000</v>
+        <v>0</v>
       </c>
       <c r="L26" s="5">
         <v>0</v>
@@ -2141,38 +2115,42 @@
         <v>0</v>
       </c>
       <c r="N26" s="5">
-        <v>77659.84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="2">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E27" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="F27" s="4">
-        <v>39379.4166666667</v>
+        <v>39241.3333333333</v>
       </c>
       <c r="G27" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I27" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="J27" s="5">
-        <v>0</v>
+        <v>6169.6</v>
       </c>
       <c r="K27" s="5">
-        <v>48000</v>
+        <v>134400</v>
       </c>
       <c r="L27" s="5">
         <v>0</v>
@@ -2181,40 +2159,42 @@
         <v>0</v>
       </c>
       <c r="N27" s="5">
-        <v>48000</v>
+        <v>140569.6</v>
       </c>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="2">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="F28" s="4">
-        <v>39386.4166666667</v>
+        <v>39323.4166666667</v>
       </c>
       <c r="G28" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I28" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="J28" s="5">
-        <v>0</v>
+        <v>1152</v>
       </c>
       <c r="K28" s="5">
-        <v>2156.06005859375</v>
+        <v>4793</v>
       </c>
       <c r="L28" s="5">
         <v>0</v>
@@ -2223,84 +2203,84 @@
         <v>0</v>
       </c>
       <c r="N28" s="5">
-        <v>2156.06005859375</v>
+        <v>5945</v>
       </c>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="2">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>124</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="E29" s="3"/>
       <c r="F29" s="4">
-        <v>39407.4166666667</v>
+        <v>39323.4166666667</v>
       </c>
       <c r="G29" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="I29" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="J29" s="5">
-        <v>0</v>
+        <v>1300.8</v>
       </c>
       <c r="K29" s="5">
-        <v>32000</v>
+        <v>31200.9609375</v>
       </c>
       <c r="L29" s="5">
-        <v>0</v>
+        <v>40.6500015258789</v>
       </c>
       <c r="M29" s="5">
-        <v>0</v>
+        <v>26016.0009765625</v>
       </c>
       <c r="N29" s="5">
-        <v>32000</v>
+        <v>58517.7619140625</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="F30" s="4">
-        <v>39414.4166666667</v>
+        <v>39323.4166666667</v>
       </c>
       <c r="G30" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="J30" s="5">
-        <v>5600</v>
+        <v>2764.8</v>
       </c>
       <c r="K30" s="5">
-        <v>83000</v>
+        <v>11651</v>
       </c>
       <c r="L30" s="5">
         <v>0</v>
@@ -2309,40 +2289,42 @@
         <v>0</v>
       </c>
       <c r="N30" s="5">
-        <v>88600</v>
+        <v>14415.8</v>
       </c>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="2">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E31" s="3"/>
+        <v>118</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="F31" s="4">
-        <v>39435.4166666667</v>
+        <v>39323.4166666667</v>
       </c>
       <c r="G31" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>125</v>
+        <v>58</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="J31" s="5">
-        <v>5040</v>
+        <v>2304</v>
       </c>
       <c r="K31" s="5">
-        <v>130000</v>
+        <v>0</v>
       </c>
       <c r="L31" s="5">
         <v>0</v>
@@ -2351,38 +2333,42 @@
         <v>0</v>
       </c>
       <c r="N31" s="5">
-        <v>135040</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="2">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E32" s="3"/>
+        <v>122</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="F32" s="4">
-        <v>39386.4166666667</v>
+        <v>39358.4166666667</v>
       </c>
       <c r="G32" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I32" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="J32" s="5">
-        <v>0</v>
+        <v>2659.84</v>
       </c>
       <c r="K32" s="5">
-        <v>87000</v>
+        <v>75000</v>
       </c>
       <c r="L32" s="5">
         <v>0</v>
@@ -2391,38 +2377,36 @@
         <v>0</v>
       </c>
       <c r="N32" s="5">
-        <v>87000</v>
+        <v>77659.84</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="2">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>123</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="4">
-        <v>39407.4166666667</v>
+        <v>42116.4652200366</v>
       </c>
       <c r="G33" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="5">
         <v>0</v>
       </c>
       <c r="K33" s="5">
-        <v>16000</v>
+        <v>0</v>
       </c>
       <c r="L33" s="5">
         <v>0</v>
@@ -2431,38 +2415,38 @@
         <v>0</v>
       </c>
       <c r="N33" s="5">
-        <v>16000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="2">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E34" s="3"/>
+        <v>127</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="F34" s="4">
-        <v>39407.4166666667</v>
+        <v>39309.4166666667</v>
       </c>
       <c r="G34" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="5">
         <v>0</v>
       </c>
       <c r="K34" s="5">
-        <v>38817.8515625</v>
+        <v>0.00999999977648258</v>
       </c>
       <c r="L34" s="5">
         <v>0</v>
@@ -2471,38 +2455,36 @@
         <v>0</v>
       </c>
       <c r="N34" s="5">
-        <v>38817.8515625</v>
+        <v>0.00999999977648258</v>
       </c>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="2">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>123</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="4">
-        <v>39407.4166666667</v>
+        <v>42116.4652200366</v>
       </c>
       <c r="G35" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="5">
         <v>0</v>
       </c>
       <c r="K35" s="5">
-        <v>33000</v>
+        <v>0</v>
       </c>
       <c r="L35" s="5">
         <v>0</v>
@@ -2511,116 +2493,126 @@
         <v>0</v>
       </c>
       <c r="N35" s="5">
-        <v>33000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="2">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="4">
         <v>39323.4166666667</v>
       </c>
       <c r="G36" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="J36" s="5">
-        <v>1300.8</v>
+        <v>1152</v>
       </c>
       <c r="K36" s="5">
-        <v>31200.9609375</v>
+        <v>4793</v>
       </c>
       <c r="L36" s="5">
-        <v>40.6500015258789</v>
+        <v>0</v>
       </c>
       <c r="M36" s="5">
-        <v>26016.0009765625</v>
+        <v>0</v>
       </c>
       <c r="N36" s="5">
-        <v>58517.7619140625</v>
+        <v>5945</v>
       </c>
     </row>
     <row r="37" spans="1:14">
       <c r="A37" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D37" s="3"/>
+        <v>134</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E37" s="3"/>
       <c r="F37" s="4">
-        <v>42115.9500275432</v>
+        <v>39323.4166666667</v>
       </c>
       <c r="G37" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I37" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="J37" s="5">
-        <v>0</v>
+        <v>1300.8</v>
       </c>
       <c r="K37" s="5">
-        <v>0</v>
+        <v>31200.9609375</v>
       </c>
       <c r="L37" s="5">
-        <v>0</v>
+        <v>40.6500015258789</v>
       </c>
       <c r="M37" s="5">
-        <v>0</v>
+        <v>26016.0009765625</v>
       </c>
       <c r="N37" s="5">
-        <v>0</v>
+        <v>58517.7619140625</v>
       </c>
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="2">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+        <v>136</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="F38" s="4">
-        <v>42115.9500275432</v>
+        <v>39323.4166666667</v>
       </c>
       <c r="G38" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I38" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="J38" s="5">
         <v>0</v>
       </c>
       <c r="K38" s="5">
-        <v>0</v>
+        <v>106140</v>
       </c>
       <c r="L38" s="5">
         <v>0</v>
@@ -2629,116 +2621,124 @@
         <v>0</v>
       </c>
       <c r="N38" s="5">
-        <v>0</v>
+        <v>106140</v>
       </c>
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="2">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D39" s="3"/>
+        <v>140</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E39" s="3"/>
       <c r="F39" s="4">
-        <v>42115.9500275432</v>
+        <v>39323.4166666667</v>
       </c>
       <c r="G39" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I39" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="J39" s="5">
-        <v>0</v>
+        <v>2764.8</v>
       </c>
       <c r="K39" s="5">
-        <v>0</v>
+        <v>11651</v>
       </c>
       <c r="L39" s="5">
-        <v>0</v>
+        <v>43.2000007629395</v>
       </c>
       <c r="M39" s="5">
-        <v>0</v>
+        <v>55296.0009765626</v>
       </c>
       <c r="N39" s="5">
-        <v>0</v>
+        <v>69711.8009765626</v>
       </c>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="2">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="4">
-        <v>39199.3333333333</v>
+        <v>39323.4166666667</v>
       </c>
       <c r="G40" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="J40" s="5">
-        <v>4608</v>
+        <v>2304</v>
       </c>
       <c r="K40" s="5">
-        <v>70779.5703125</v>
+        <v>0</v>
       </c>
       <c r="L40" s="5">
-        <v>40.2999992370605</v>
+        <v>0</v>
       </c>
       <c r="M40" s="5">
-        <v>25791.9995117187</v>
+        <v>0</v>
       </c>
       <c r="N40" s="5">
-        <v>101179.569824219</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="2">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+        <v>144</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>146</v>
+      </c>
       <c r="F41" s="4">
-        <v>42115.9500275432</v>
+        <v>39344.4166666667</v>
       </c>
       <c r="G41" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="5">
         <v>0</v>
       </c>
       <c r="K41" s="5">
-        <v>0</v>
+        <v>0.00999999977648258</v>
       </c>
       <c r="L41" s="5">
         <v>0</v>
@@ -2747,40 +2747,42 @@
         <v>0</v>
       </c>
       <c r="N41" s="5">
-        <v>0</v>
+        <v>0.00999999977648258</v>
       </c>
     </row>
     <row r="42" spans="1:14">
       <c r="A42" s="2">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E42" s="3"/>
+        <v>137</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="F42" s="4">
-        <v>39323.4166666667</v>
+        <v>39351.4166666667</v>
       </c>
       <c r="G42" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="J42" s="5">
-        <v>2304</v>
+        <v>2659.84</v>
       </c>
       <c r="K42" s="5">
-        <v>0</v>
+        <v>72500</v>
       </c>
       <c r="L42" s="5">
         <v>0</v>
@@ -2789,40 +2791,36 @@
         <v>0</v>
       </c>
       <c r="N42" s="5">
-        <v>2304</v>
+        <v>75159.84</v>
       </c>
     </row>
     <row r="43" spans="1:14">
       <c r="A43" s="2">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>85</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="4">
-        <v>39323.4166666667</v>
+        <v>42116.4652200366</v>
       </c>
       <c r="G43" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>97</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I43" s="3"/>
       <c r="J43" s="5">
-        <v>1152</v>
+        <v>0</v>
       </c>
       <c r="K43" s="5">
-        <v>4793</v>
+        <v>0</v>
       </c>
       <c r="L43" s="5">
         <v>0</v>
@@ -2831,7 +2829,7 @@
         <v>0</v>
       </c>
       <c r="N43" s="5">
-        <v>5945</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2839,26 +2837,26 @@
         <v>53</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="4">
         <v>39323.4166666667</v>
       </c>
       <c r="G44" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="J44" s="5">
         <v>1152</v>
@@ -2878,35 +2876,35 @@
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="4">
         <v>39323.4166666667</v>
       </c>
       <c r="G45" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="J45" s="5">
-        <v>2304</v>
+        <v>1300.8</v>
       </c>
       <c r="K45" s="5">
-        <v>0</v>
+        <v>31200.9609375</v>
       </c>
       <c r="L45" s="5">
         <v>0</v>
@@ -2915,40 +2913,42 @@
         <v>0</v>
       </c>
       <c r="N45" s="5">
-        <v>2304</v>
+        <v>32501.7609375</v>
       </c>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E46" s="3"/>
+        <v>155</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>160</v>
+      </c>
       <c r="F46" s="4">
         <v>39323.4166666667</v>
       </c>
       <c r="G46" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>86</v>
+        <v>161</v>
       </c>
       <c r="J46" s="5">
-        <v>1300.8</v>
+        <v>0</v>
       </c>
       <c r="K46" s="5">
-        <v>31200.9609375</v>
+        <v>46116</v>
       </c>
       <c r="L46" s="5">
         <v>0</v>
@@ -2957,42 +2957,40 @@
         <v>0</v>
       </c>
       <c r="N46" s="5">
-        <v>32501.7609375</v>
+        <v>46116</v>
       </c>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="2">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>168</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="E47" s="3"/>
       <c r="F47" s="4">
         <v>39323.4166666667</v>
       </c>
       <c r="G47" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="J47" s="5">
-        <v>0</v>
+        <v>2048</v>
       </c>
       <c r="K47" s="5">
-        <v>46116</v>
+        <v>11651</v>
       </c>
       <c r="L47" s="5">
         <v>0</v>
@@ -3001,42 +2999,40 @@
         <v>0</v>
       </c>
       <c r="N47" s="5">
-        <v>46116</v>
+        <v>13699</v>
       </c>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="2">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>172</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="E48" s="3"/>
       <c r="F48" s="4">
-        <v>39351.4166666667</v>
+        <v>39323.4166666667</v>
       </c>
       <c r="G48" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="J48" s="5">
-        <v>2659.84</v>
+        <v>2304</v>
       </c>
       <c r="K48" s="5">
-        <v>72500</v>
+        <v>0</v>
       </c>
       <c r="L48" s="5">
         <v>0</v>
@@ -3045,42 +3041,40 @@
         <v>0</v>
       </c>
       <c r="N48" s="5">
-        <v>75159.84</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="49" spans="1:14">
       <c r="A49" s="2">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F49" s="4">
-        <v>39351.4166666667</v>
+        <v>39344.4166666667</v>
       </c>
       <c r="G49" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>113</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="I49" s="3"/>
       <c r="J49" s="5">
-        <v>2659.84</v>
+        <v>0</v>
       </c>
       <c r="K49" s="5">
-        <v>31500</v>
+        <v>0.00999999977648258</v>
       </c>
       <c r="L49" s="5">
         <v>0</v>
@@ -3089,42 +3083,42 @@
         <v>0</v>
       </c>
       <c r="N49" s="5">
-        <v>34159.84</v>
+        <v>0.00999999977648258</v>
       </c>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" s="2">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>85</v>
+        <v>172</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>93</v>
+        <v>150</v>
       </c>
       <c r="F50" s="4">
-        <v>39323.4166666667</v>
+        <v>39351.4166666667</v>
       </c>
       <c r="G50" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>178</v>
+        <v>124</v>
       </c>
       <c r="J50" s="5">
-        <v>2764.8</v>
+        <v>2659.84</v>
       </c>
       <c r="K50" s="5">
-        <v>11651</v>
+        <v>31500</v>
       </c>
       <c r="L50" s="5">
         <v>0</v>
@@ -3133,82 +3127,80 @@
         <v>0</v>
       </c>
       <c r="N50" s="5">
-        <v>14415.8</v>
+        <v>34159.84</v>
       </c>
     </row>
     <row r="51" spans="1:14">
       <c r="A51" s="2">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>85</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="4">
-        <v>39323.4166666667</v>
+        <v>42116.4652200366</v>
       </c>
       <c r="G51" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>178</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I51" s="3"/>
       <c r="J51" s="5">
-        <v>2764.8</v>
+        <v>0</v>
       </c>
       <c r="K51" s="5">
-        <v>11651</v>
+        <v>0</v>
       </c>
       <c r="L51" s="5">
-        <v>43.2000007629395</v>
+        <v>0</v>
       </c>
       <c r="M51" s="5">
-        <v>55296.0009765626</v>
+        <v>0</v>
       </c>
       <c r="N51" s="5">
-        <v>69711.8009765626</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:14">
       <c r="A52" s="2">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E52" s="3"/>
+        <v>177</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="F52" s="4">
-        <v>39323.4166666667</v>
+        <v>39351.4166666667</v>
       </c>
       <c r="G52" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>94</v>
+        <v>178</v>
       </c>
       <c r="J52" s="5">
-        <v>2048</v>
+        <v>4965.6</v>
       </c>
       <c r="K52" s="5">
-        <v>11651</v>
+        <v>8642</v>
       </c>
       <c r="L52" s="5">
         <v>0</v>
@@ -3217,36 +3209,38 @@
         <v>0</v>
       </c>
       <c r="N52" s="5">
-        <v>13699</v>
+        <v>13607.6</v>
       </c>
     </row>
     <row r="53" spans="1:14">
       <c r="A53" s="2">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D53" s="3"/>
+        <v>180</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E53" s="3"/>
       <c r="F53" s="4">
-        <v>42115.9500275432</v>
+        <v>39379.4166666667</v>
       </c>
       <c r="G53" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="5">
         <v>0</v>
       </c>
       <c r="K53" s="5">
-        <v>0</v>
+        <v>48000</v>
       </c>
       <c r="L53" s="5">
         <v>0</v>
@@ -3255,36 +3249,38 @@
         <v>0</v>
       </c>
       <c r="N53" s="5">
-        <v>0</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="54" spans="1:14">
       <c r="A54" s="2">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D54" s="3"/>
+        <v>183</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>184</v>
+      </c>
       <c r="E54" s="3"/>
       <c r="F54" s="4">
-        <v>42115.9500275432</v>
+        <v>39386.4166666667</v>
       </c>
       <c r="G54" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="I54" s="3"/>
       <c r="J54" s="5">
         <v>0</v>
       </c>
       <c r="K54" s="5">
-        <v>0</v>
+        <v>87000</v>
       </c>
       <c r="L54" s="5">
         <v>0</v>
@@ -3293,36 +3289,40 @@
         <v>0</v>
       </c>
       <c r="N54" s="5">
-        <v>0</v>
+        <v>87000</v>
       </c>
     </row>
     <row r="55" spans="1:14">
       <c r="A55" s="2">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
       <c r="F55" s="4">
-        <v>42115.9500275432</v>
+        <v>39386.4166666667</v>
       </c>
       <c r="G55" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="I55" s="3"/>
       <c r="J55" s="5">
         <v>0</v>
       </c>
       <c r="K55" s="5">
-        <v>0</v>
+        <v>2156.06005859375</v>
       </c>
       <c r="L55" s="5">
         <v>0</v>
@@ -3331,36 +3331,38 @@
         <v>0</v>
       </c>
       <c r="N55" s="5">
-        <v>0</v>
+        <v>2156.06005859375</v>
       </c>
     </row>
     <row r="56" spans="1:14">
       <c r="A56" s="2">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="4">
-        <v>42115.9500275432</v>
+        <v>39407.4166666667</v>
       </c>
       <c r="G56" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="I56" s="3"/>
       <c r="J56" s="5">
         <v>0</v>
       </c>
       <c r="K56" s="5">
-        <v>0</v>
+        <v>33000</v>
       </c>
       <c r="L56" s="5">
         <v>0</v>
@@ -3369,36 +3371,38 @@
         <v>0</v>
       </c>
       <c r="N56" s="5">
-        <v>0</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="57" spans="1:14">
       <c r="A57" s="2">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D57" s="3"/>
+        <v>192</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="E57" s="3"/>
       <c r="F57" s="4">
-        <v>42115.9500275432</v>
+        <v>39407.4166666667</v>
       </c>
       <c r="G57" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="5">
         <v>0</v>
       </c>
       <c r="K57" s="5">
-        <v>0</v>
+        <v>16000</v>
       </c>
       <c r="L57" s="5">
         <v>0</v>
@@ -3407,40 +3411,38 @@
         <v>0</v>
       </c>
       <c r="N57" s="5">
-        <v>0</v>
+        <v>16000</v>
       </c>
     </row>
     <row r="58" spans="1:14">
       <c r="A58" s="2">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>195</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="E58" s="3"/>
       <c r="F58" s="4">
-        <v>39344.4166666667</v>
+        <v>39407.4166666667</v>
       </c>
       <c r="G58" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="5">
         <v>0</v>
       </c>
       <c r="K58" s="5">
-        <v>0.00999999977648258</v>
+        <v>38817.8515625</v>
       </c>
       <c r="L58" s="5">
         <v>0</v>
@@ -3449,40 +3451,40 @@
         <v>0</v>
       </c>
       <c r="N58" s="5">
-        <v>0.00999999977648258</v>
+        <v>38817.8515625</v>
       </c>
     </row>
     <row r="59" spans="1:14">
       <c r="A59" s="2">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="D59" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>199</v>
-      </c>
       <c r="F59" s="4">
-        <v>39344.4166666667</v>
+        <v>39407.4166666667</v>
       </c>
       <c r="G59" s="4">
-        <v>42125.9500275435</v>
+        <v>42126.4652200368</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="I59" s="3"/>
       <c r="J59" s="5">
         <v>0</v>
       </c>
       <c r="K59" s="5">
-        <v>0.00999999977648258</v>
+        <v>32000</v>
       </c>
       <c r="L59" s="5">
         <v>0</v>
@@ -3491,51 +3493,93 @@
         <v>0</v>
       </c>
       <c r="N59" s="5">
-        <v>0.00999999977648258</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="60" spans="1:14">
       <c r="A60" s="2">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E60" s="3" t="s">
+      <c r="F60" s="4">
+        <v>39414.4166666667</v>
+      </c>
+      <c r="G60" s="4">
+        <v>42126.4652200368</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I60" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F60" s="4">
-        <v>39062.3333333333</v>
-      </c>
-      <c r="G60" s="4">
-        <v>42125.9500275435</v>
-      </c>
-      <c r="H60" s="3" t="s">
+      <c r="J60" s="5">
+        <v>5600</v>
+      </c>
+      <c r="K60" s="5">
+        <v>83000</v>
+      </c>
+      <c r="L60" s="5">
+        <v>0</v>
+      </c>
+      <c r="M60" s="5">
+        <v>0</v>
+      </c>
+      <c r="N60" s="5">
+        <v>88600</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="2">
+        <v>40</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="I60" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J60" s="5">
-        <v>616.96</v>
-      </c>
-      <c r="K60" s="5">
-        <v>2000</v>
-      </c>
-      <c r="L60" s="5">
-        <v>0</v>
-      </c>
-      <c r="M60" s="5">
-        <v>0</v>
-      </c>
-      <c r="N60" s="5">
-        <v>2616.96</v>
+      <c r="C61" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E61" s="3"/>
+      <c r="F61" s="4">
+        <v>39435.4166666667</v>
+      </c>
+      <c r="G61" s="4">
+        <v>42126.4652200368</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="J61" s="5">
+        <v>5040</v>
+      </c>
+      <c r="K61" s="5">
+        <v>130000</v>
+      </c>
+      <c r="L61" s="5">
+        <v>0</v>
+      </c>
+      <c r="M61" s="5">
+        <v>0</v>
+      </c>
+      <c r="N61" s="5">
+        <v>135040</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Activity groups total/resource cost
</commit_message>
<xml_diff>
--- a/PMConverter/src/test_alexander.xlsx
+++ b/PMConverter/src/test_alexander.xlsx
@@ -1133,10 +1133,10 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4">
-        <v>42116.4652200366</v>
+        <v>42116.6117988432</v>
       </c>
       <c r="G3" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>20</v>
@@ -1146,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="5">
-        <v>0</v>
+        <v>2700210.30574707</v>
       </c>
       <c r="L3" s="5">
         <v>0</v>
@@ -1155,7 +1155,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="5">
-        <v>0</v>
+        <v>2952108.70818848</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1171,10 +1171,10 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4">
-        <v>42116.4652200366</v>
+        <v>42116.6117988432</v>
       </c>
       <c r="G4" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>20</v>
@@ -1184,7 +1184,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="5">
-        <v>0</v>
+        <v>2700210.30574707</v>
       </c>
       <c r="L4" s="5">
         <v>0</v>
@@ -1193,7 +1193,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="5">
-        <v>0</v>
+        <v>2952108.70818848</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1214,7 +1214,7 @@
         <v>38824.3333333333</v>
       </c>
       <c r="G5" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>26</v>
@@ -1256,7 +1256,7 @@
         <v>38908.3333333333</v>
       </c>
       <c r="G6" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>31</v>
@@ -1294,7 +1294,7 @@
         <v>38824.3333333333</v>
       </c>
       <c r="G7" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>31</v>
@@ -1332,7 +1332,7 @@
         <v>38824.3333333333</v>
       </c>
       <c r="G8" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>26</v>
@@ -1374,7 +1374,7 @@
         <v>38936.3333333333</v>
       </c>
       <c r="G9" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>26</v>
@@ -1416,7 +1416,7 @@
         <v>39020.3333333333</v>
       </c>
       <c r="G10" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>20</v>
@@ -1453,10 +1453,10 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4">
-        <v>42116.4652200366</v>
+        <v>42116.6117988432</v>
       </c>
       <c r="G11" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>20</v>
@@ -1466,7 +1466,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="5">
-        <v>0</v>
+        <v>2700210.30574707</v>
       </c>
       <c r="L11" s="5">
         <v>0</v>
@@ -1475,7 +1475,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="5">
-        <v>0</v>
+        <v>2952108.70818848</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1498,7 +1498,7 @@
         <v>39062.3333333333</v>
       </c>
       <c r="G12" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>48</v>
@@ -1542,7 +1542,7 @@
         <v>39062.3333333333</v>
       </c>
       <c r="G13" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>53</v>
@@ -1586,7 +1586,7 @@
         <v>39080.3333333333</v>
       </c>
       <c r="G14" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>58</v>
@@ -1630,7 +1630,7 @@
         <v>39080.3333333333</v>
       </c>
       <c r="G15" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>64</v>
@@ -1674,7 +1674,7 @@
         <v>39094.3333333333</v>
       </c>
       <c r="G16" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>68</v>
@@ -1711,10 +1711,10 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="4">
-        <v>42116.4652200366</v>
+        <v>42116.6117988432</v>
       </c>
       <c r="G17" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>20</v>
@@ -1724,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="5">
-        <v>0</v>
+        <v>2700210.30574707</v>
       </c>
       <c r="L17" s="5">
         <v>0</v>
@@ -1733,7 +1733,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="5">
-        <v>0</v>
+        <v>2952108.70818848</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1756,7 +1756,7 @@
         <v>39115.3333333333</v>
       </c>
       <c r="G18" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>31</v>
@@ -1800,7 +1800,7 @@
         <v>39143.3333333333</v>
       </c>
       <c r="G19" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>64</v>
@@ -1844,7 +1844,7 @@
         <v>39157.3333333333</v>
       </c>
       <c r="G20" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>82</v>
@@ -1888,7 +1888,7 @@
         <v>39178.3333333333</v>
       </c>
       <c r="G21" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>82</v>
@@ -1925,10 +1925,10 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="4">
-        <v>42116.4652200366</v>
+        <v>42116.6117988432</v>
       </c>
       <c r="G22" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>20</v>
@@ -1938,7 +1938,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="5">
-        <v>0</v>
+        <v>2700210.30574707</v>
       </c>
       <c r="L22" s="5">
         <v>0</v>
@@ -1947,7 +1947,7 @@
         <v>0</v>
       </c>
       <c r="N22" s="5">
-        <v>0</v>
+        <v>2952108.70818848</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1970,7 +1970,7 @@
         <v>39199.3333333333</v>
       </c>
       <c r="G23" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>31</v>
@@ -2014,7 +2014,7 @@
         <v>39227.3333333333</v>
       </c>
       <c r="G24" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>64</v>
@@ -2056,7 +2056,7 @@
         <v>39199.3333333333</v>
       </c>
       <c r="G25" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>64</v>
@@ -2093,10 +2093,10 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="4">
-        <v>42116.4652200366</v>
+        <v>42116.6117988432</v>
       </c>
       <c r="G26" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>20</v>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="5">
-        <v>0</v>
+        <v>2700210.30574707</v>
       </c>
       <c r="L26" s="5">
         <v>0</v>
@@ -2115,7 +2115,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="5">
-        <v>0</v>
+        <v>2952108.70818848</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -2138,7 +2138,7 @@
         <v>39241.3333333333</v>
       </c>
       <c r="G27" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>64</v>
@@ -2182,7 +2182,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G28" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>64</v>
@@ -2224,7 +2224,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G29" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>64</v>
@@ -2268,7 +2268,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G30" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>31</v>
@@ -2312,7 +2312,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G31" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>58</v>
@@ -2356,7 +2356,7 @@
         <v>39358.4166666667</v>
       </c>
       <c r="G32" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>31</v>
@@ -2393,10 +2393,10 @@
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="4">
-        <v>42116.4652200366</v>
+        <v>42116.6117988432</v>
       </c>
       <c r="G33" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>20</v>
@@ -2406,7 +2406,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="5">
-        <v>0</v>
+        <v>2700210.30574707</v>
       </c>
       <c r="L33" s="5">
         <v>0</v>
@@ -2415,7 +2415,7 @@
         <v>0</v>
       </c>
       <c r="N33" s="5">
-        <v>0</v>
+        <v>2952108.70818848</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -2436,7 +2436,7 @@
         <v>39309.4166666667</v>
       </c>
       <c r="G34" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>64</v>
@@ -2471,10 +2471,10 @@
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="4">
-        <v>42116.4652200366</v>
+        <v>42116.6117988432</v>
       </c>
       <c r="G35" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>20</v>
@@ -2484,7 +2484,7 @@
         <v>0</v>
       </c>
       <c r="K35" s="5">
-        <v>0</v>
+        <v>2700210.30574707</v>
       </c>
       <c r="L35" s="5">
         <v>0</v>
@@ -2493,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="N35" s="5">
-        <v>0</v>
+        <v>2952108.70818848</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -2514,7 +2514,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G36" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>64</v>
@@ -2556,7 +2556,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G37" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>64</v>
@@ -2600,7 +2600,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G38" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>82</v>
@@ -2642,7 +2642,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G39" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>31</v>
@@ -2684,7 +2684,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G40" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>58</v>
@@ -2728,7 +2728,7 @@
         <v>39344.4166666667</v>
       </c>
       <c r="G41" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>147</v>
@@ -2770,7 +2770,7 @@
         <v>39351.4166666667</v>
       </c>
       <c r="G42" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>31</v>
@@ -2807,10 +2807,10 @@
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="4">
-        <v>42116.4652200366</v>
+        <v>42116.6117988432</v>
       </c>
       <c r="G43" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>20</v>
@@ -2820,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="K43" s="5">
-        <v>0</v>
+        <v>2700210.30574707</v>
       </c>
       <c r="L43" s="5">
         <v>0</v>
@@ -2829,7 +2829,7 @@
         <v>0</v>
       </c>
       <c r="N43" s="5">
-        <v>0</v>
+        <v>2952108.70818848</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2850,7 +2850,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G44" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>64</v>
@@ -2892,7 +2892,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G45" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>64</v>
@@ -2936,7 +2936,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G46" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>82</v>
@@ -2978,7 +2978,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G47" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>31</v>
@@ -3020,7 +3020,7 @@
         <v>39323.4166666667</v>
       </c>
       <c r="G48" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>58</v>
@@ -3064,7 +3064,7 @@
         <v>39344.4166666667</v>
       </c>
       <c r="G49" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>147</v>
@@ -3106,7 +3106,7 @@
         <v>39351.4166666667</v>
       </c>
       <c r="G50" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>31</v>
@@ -3143,10 +3143,10 @@
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="4">
-        <v>42116.4652200366</v>
+        <v>42116.6117988432</v>
       </c>
       <c r="G51" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>20</v>
@@ -3156,7 +3156,7 @@
         <v>0</v>
       </c>
       <c r="K51" s="5">
-        <v>0</v>
+        <v>2700210.30574707</v>
       </c>
       <c r="L51" s="5">
         <v>0</v>
@@ -3165,7 +3165,7 @@
         <v>0</v>
       </c>
       <c r="N51" s="5">
-        <v>0</v>
+        <v>2952108.70818848</v>
       </c>
     </row>
     <row r="52" spans="1:14">
@@ -3188,7 +3188,7 @@
         <v>39351.4166666667</v>
       </c>
       <c r="G52" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>82</v>
@@ -3230,7 +3230,7 @@
         <v>39379.4166666667</v>
       </c>
       <c r="G53" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>58</v>
@@ -3270,7 +3270,7 @@
         <v>39386.4166666667</v>
       </c>
       <c r="G54" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>82</v>
@@ -3312,7 +3312,7 @@
         <v>39386.4166666667</v>
       </c>
       <c r="G55" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>82</v>
@@ -3352,7 +3352,7 @@
         <v>39407.4166666667</v>
       </c>
       <c r="G56" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>64</v>
@@ -3392,7 +3392,7 @@
         <v>39407.4166666667</v>
       </c>
       <c r="G57" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>64</v>
@@ -3432,7 +3432,7 @@
         <v>39407.4166666667</v>
       </c>
       <c r="G58" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>147</v>
@@ -3474,7 +3474,7 @@
         <v>39407.4166666667</v>
       </c>
       <c r="G59" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H59" s="3" t="s">
         <v>147</v>
@@ -3516,7 +3516,7 @@
         <v>39414.4166666667</v>
       </c>
       <c r="G60" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>82</v>
@@ -3558,7 +3558,7 @@
         <v>39435.4166666667</v>
       </c>
       <c r="G61" s="4">
-        <v>42126.4652200368</v>
+        <v>42126.6117988434</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>147</v>

</xml_diff>